<commit_message>
Example and Readme cupdates
</commit_message>
<xml_diff>
--- a/Example/Example_project/Info2.xlsx
+++ b/Example/Example_project/Info2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nms198_newcastle_ac_uk/Documents/3_Coding/Git/TimeSeriesProcessor/Example/Example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="823" documentId="6_{9E37F347-3A89-43C3-83FF-EA444BC37A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5FFF357-9ACB-4C66-87D8-49406E93CDEE}"/>
+  <xr:revisionPtr revIDLastSave="921" documentId="6_{9E37F347-3A89-43C3-83FF-EA444BC37A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{921A13EC-D081-42EC-9C20-C1D961F49B9E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="9" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="page_sizes" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">parameters!$A$1:$R$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">parameters_ave!$A$1:$Q$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">parameters!$A$1:$R$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">parameters_ave!$A$1:$P$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">plots!$A$1:$F$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="219">
   <si>
     <t>plot</t>
   </si>
@@ -242,48 +242,18 @@
     <t>BOD5</t>
   </si>
   <si>
-    <t>BOD5_1</t>
-  </si>
-  <si>
-    <t>BOD5_ave</t>
-  </si>
-  <si>
     <t>BOD</t>
   </si>
   <si>
-    <t>BOD5_2</t>
-  </si>
-  <si>
-    <t>BOD5_3</t>
-  </si>
-  <si>
     <t>tCOD</t>
   </si>
   <si>
-    <t>tCOD_1</t>
-  </si>
-  <si>
-    <t>tCOD_ave</t>
-  </si>
-  <si>
     <t>COD</t>
   </si>
   <si>
-    <t>tCOD_2</t>
-  </si>
-  <si>
     <t>sCOD</t>
   </si>
   <si>
-    <t>sCOD_1</t>
-  </si>
-  <si>
-    <t>sCOD_ave</t>
-  </si>
-  <si>
-    <t>sCOD_2</t>
-  </si>
-  <si>
     <t>circle</t>
   </si>
   <si>
@@ -311,9 +281,6 @@
     <t>selected_plot_set_1</t>
   </si>
   <si>
-    <t>selected_plot_set_2</t>
-  </si>
-  <si>
     <t>Average Voltage&lt;br&gt;(mV)</t>
   </si>
   <si>
@@ -398,12 +365,6 @@
     <t>SampleLog</t>
   </si>
   <si>
-    <t>C:/path/to/TS_data/</t>
-  </si>
-  <si>
-    <t>C:/path/to/Sample_data/</t>
-  </si>
-  <si>
     <t>expt</t>
   </si>
   <si>
@@ -512,27 +473,6 @@
     <t>2_V_ave</t>
   </si>
   <si>
-    <t>BOD₅ 1</t>
-  </si>
-  <si>
-    <t>BOD₅ 2</t>
-  </si>
-  <si>
-    <t>BOD₅ 3</t>
-  </si>
-  <si>
-    <t>tCOD 1</t>
-  </si>
-  <si>
-    <t>tCOD 2</t>
-  </si>
-  <si>
-    <t>sCOD 1</t>
-  </si>
-  <si>
-    <t>sCOD 2</t>
-  </si>
-  <si>
     <t>Heater A Enabled</t>
   </si>
   <si>
@@ -575,7 +515,193 @@
     <t>Stage 2 (ave)</t>
   </si>
   <si>
-    <t>BOD₅</t>
+    <t>Example/Example_Sample_data</t>
+  </si>
+  <si>
+    <t>Example/Example_TS_data</t>
+  </si>
+  <si>
+    <t>A_BOD5_1</t>
+  </si>
+  <si>
+    <t>A_BOD5_2</t>
+  </si>
+  <si>
+    <t>A_BOD5_3</t>
+  </si>
+  <si>
+    <t>A_tCOD_1</t>
+  </si>
+  <si>
+    <t>A_tCOD_2</t>
+  </si>
+  <si>
+    <t>A_sCOD_1</t>
+  </si>
+  <si>
+    <t>A_sCOD_2</t>
+  </si>
+  <si>
+    <t>A_BOD5_ave</t>
+  </si>
+  <si>
+    <t>A_tCOD_ave</t>
+  </si>
+  <si>
+    <t>A_sCOD_ave</t>
+  </si>
+  <si>
+    <t>A BOD₅ 1</t>
+  </si>
+  <si>
+    <t>A BOD₅ 2</t>
+  </si>
+  <si>
+    <t>A BOD₅ 3</t>
+  </si>
+  <si>
+    <t>A tCOD 1</t>
+  </si>
+  <si>
+    <t>A tCOD 2</t>
+  </si>
+  <si>
+    <t>A sCOD 1</t>
+  </si>
+  <si>
+    <t>A sCOD 2</t>
+  </si>
+  <si>
+    <t>B_BOD5_1</t>
+  </si>
+  <si>
+    <t>B_BOD5_ave</t>
+  </si>
+  <si>
+    <t>B_BOD5_2</t>
+  </si>
+  <si>
+    <t>B_BOD5_3</t>
+  </si>
+  <si>
+    <t>B_tCOD_1</t>
+  </si>
+  <si>
+    <t>B_tCOD_ave</t>
+  </si>
+  <si>
+    <t>B_tCOD_2</t>
+  </si>
+  <si>
+    <t>B_sCOD_1</t>
+  </si>
+  <si>
+    <t>B_sCOD_ave</t>
+  </si>
+  <si>
+    <t>B_sCOD_2</t>
+  </si>
+  <si>
+    <t>B BOD₅ 1</t>
+  </si>
+  <si>
+    <t>B BOD₅ 2</t>
+  </si>
+  <si>
+    <t>B BOD₅ 3</t>
+  </si>
+  <si>
+    <t>B tCOD 1</t>
+  </si>
+  <si>
+    <t>B tCOD 2</t>
+  </si>
+  <si>
+    <t>B sCOD 1</t>
+  </si>
+  <si>
+    <t>B sCOD 2</t>
+  </si>
+  <si>
+    <t>C BOD₅ 1</t>
+  </si>
+  <si>
+    <t>C BOD₅ 2</t>
+  </si>
+  <si>
+    <t>C BOD₅ 3</t>
+  </si>
+  <si>
+    <t>C tCOD 1</t>
+  </si>
+  <si>
+    <t>C tCOD 2</t>
+  </si>
+  <si>
+    <t>C sCOD 1</t>
+  </si>
+  <si>
+    <t>C sCOD 2</t>
+  </si>
+  <si>
+    <t>C_BOD5_1</t>
+  </si>
+  <si>
+    <t>C_BOD5_ave</t>
+  </si>
+  <si>
+    <t>C_BOD5_2</t>
+  </si>
+  <si>
+    <t>C_BOD5_3</t>
+  </si>
+  <si>
+    <t>C_tCOD_1</t>
+  </si>
+  <si>
+    <t>C_tCOD_ave</t>
+  </si>
+  <si>
+    <t>C_tCOD_2</t>
+  </si>
+  <si>
+    <t>C_sCOD_1</t>
+  </si>
+  <si>
+    <t>C_sCOD_ave</t>
+  </si>
+  <si>
+    <t>C_sCOD_2</t>
+  </si>
+  <si>
+    <t>A BOD₅</t>
+  </si>
+  <si>
+    <t>A tCOD</t>
+  </si>
+  <si>
+    <t>A sCOD</t>
+  </si>
+  <si>
+    <t>B BOD₅</t>
+  </si>
+  <si>
+    <t>B tCOD</t>
+  </si>
+  <si>
+    <t>B sCOD</t>
+  </si>
+  <si>
+    <t>C BOD₅</t>
+  </si>
+  <si>
+    <t>C tCOD</t>
+  </si>
+  <si>
+    <t>C sCOD</t>
+  </si>
+  <si>
+    <t>Reactor Temp (ave)</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1288,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,7 +1310,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1200,12 +1326,12 @@
         <v>17</v>
       </c>
       <c r="B4" s="36">
-        <v>44941.5</v>
+        <v>44947</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1213,7 +1339,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -1230,7 +1356,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,13 +1396,13 @@
     </row>
     <row r="2" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B2" s="37">
         <v>1</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="E2" s="39" t="s">
         <v>23</v>
@@ -1287,13 +1413,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -1344,22 +1470,22 @@
         <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="J1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="K1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="L1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1367,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -1399,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1431,10 +1557,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1465,10 +1591,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E5" s="42">
         <v>44566.375</v>
@@ -1503,7 +1629,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1574,18 +1700,18 @@
         <v>58</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1602,10 +1728,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1622,10 +1748,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1642,20 +1768,20 @@
     </row>
     <row r="5" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1675,10 +1801,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1724,10 +1850,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1763,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33:R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1838,30 +1964,30 @@
         <v>49</v>
       </c>
       <c r="Q1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="R1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
@@ -1876,10 +2002,10 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>2</v>
@@ -1896,22 +2022,22 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
-        <v>128</v>
-      </c>
       <c r="C3" s="47" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G3" t="s">
         <v>61</v>
@@ -1946,22 +2072,22 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
         <v>61</v>
@@ -1976,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" t="s">
         <v>2</v>
@@ -1996,22 +2122,22 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
         <v>61</v>
@@ -2026,10 +2152,10 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N5" t="s">
         <v>2</v>
@@ -2046,22 +2172,22 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
@@ -2076,10 +2202,10 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L6" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N6" t="s">
         <v>2</v>
@@ -2096,22 +2222,22 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G7" t="s">
         <v>61</v>
@@ -2126,10 +2252,10 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L7" s="49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N7" t="s">
         <v>2</v>
@@ -2145,23 +2271,23 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
-        <v>116</v>
+      <c r="A8" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
       </c>
       <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -2172,22 +2298,22 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
+        <v>159</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -2198,22 +2324,22 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
+        <v>160</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2224,22 +2350,22 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2250,22 +2376,22 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
+        <v>162</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -2276,22 +2402,22 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="41" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -2302,387 +2428,751 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>77</v>
+        <v>164</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>167</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q15" s="49">
+        <v>0</v>
+      </c>
+      <c r="R15" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q16" s="49">
+        <v>0</v>
+      </c>
+      <c r="R16" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" s="49">
+        <v>0</v>
+      </c>
+      <c r="R17" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q18" s="49">
+        <v>0</v>
+      </c>
+      <c r="R18" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q19" s="49">
+        <v>0</v>
+      </c>
+      <c r="R19" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" s="49">
+        <v>0</v>
+      </c>
+      <c r="R20" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>191</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q21" s="49">
+        <v>0</v>
+      </c>
+      <c r="R21" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q22" s="49">
+        <v>0</v>
+      </c>
+      <c r="R22" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q23" s="49">
+        <v>0</v>
+      </c>
+      <c r="R23" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q24" s="49">
+        <v>0</v>
+      </c>
+      <c r="R24" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q25" s="49">
+        <v>0</v>
+      </c>
+      <c r="R25" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q26" s="49">
+        <v>0</v>
+      </c>
+      <c r="R26" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q27" s="49">
+        <v>0</v>
+      </c>
+      <c r="R27" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q28" s="49">
+        <v>0</v>
+      </c>
+      <c r="R28" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="46" t="s">
+      <c r="H29" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="49">
+        <v>19</v>
+      </c>
+      <c r="L29" s="49">
+        <v>19</v>
+      </c>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="49">
+        <v>1</v>
+      </c>
+      <c r="R29" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" s="45">
+        <v>1</v>
+      </c>
+      <c r="L30" s="45">
+        <v>1</v>
+      </c>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" s="44">
+        <v>3</v>
+      </c>
+      <c r="P30" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="44">
+        <v>1</v>
+      </c>
+      <c r="R30" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="47" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" s="48">
+        <v>2</v>
+      </c>
+      <c r="L31" s="48">
+        <v>2</v>
+      </c>
+      <c r="N31" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="O31" s="47">
+        <v>2</v>
+      </c>
+      <c r="P31" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="47">
+        <v>1</v>
+      </c>
+      <c r="R31" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="47" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" s="48">
+        <v>4</v>
+      </c>
+      <c r="L32" s="48">
+        <v>4</v>
+      </c>
+      <c r="N32" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" s="47">
+        <v>1</v>
+      </c>
+      <c r="P32" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="47">
+        <v>1</v>
+      </c>
+      <c r="R32" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" s="46" t="s">
+      <c r="C33" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="48">
+        <v>1</v>
+      </c>
+      <c r="L33" s="48">
+        <v>1</v>
+      </c>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="47">
+        <v>0</v>
+      </c>
+      <c r="R33" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="C34" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" s="49">
-        <v>19</v>
-      </c>
-      <c r="L15" s="49">
-        <v>19</v>
-      </c>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49" t="s">
+      <c r="G34" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" s="48">
         <v>2</v>
       </c>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="49">
-        <v>1</v>
-      </c>
-      <c r="R15" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" s="44" t="s">
+      <c r="L34" s="48">
+        <v>2</v>
+      </c>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="47">
+        <v>0</v>
+      </c>
+      <c r="R34" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="44" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="45">
-        <v>1</v>
-      </c>
-      <c r="L16" s="45">
-        <v>1</v>
-      </c>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44" t="s">
+      <c r="E35" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" s="48">
+        <v>4</v>
+      </c>
+      <c r="L35" s="48">
+        <v>4</v>
+      </c>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="44">
-        <v>3</v>
-      </c>
-      <c r="P16" s="44" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="44">
-        <v>1</v>
-      </c>
-      <c r="R16" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" s="47" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" s="48">
-        <v>1</v>
-      </c>
-      <c r="L17" s="48">
-        <v>1</v>
-      </c>
-      <c r="N17" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="O17" s="47">
-        <v>2</v>
-      </c>
-      <c r="P17" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="47">
-        <v>1</v>
-      </c>
-      <c r="R17" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="47" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" s="48">
-        <v>1</v>
-      </c>
-      <c r="L18" s="48">
-        <v>1</v>
-      </c>
-      <c r="N18" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="O18" s="47">
-        <v>1</v>
-      </c>
-      <c r="P18" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="47">
-        <v>1</v>
-      </c>
-      <c r="R18" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" s="48">
-        <v>1</v>
-      </c>
-      <c r="L19" s="48">
-        <v>1</v>
-      </c>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="47">
-        <v>0</v>
-      </c>
-      <c r="R19" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" s="48">
-        <v>2</v>
-      </c>
-      <c r="L20" s="48">
-        <v>2</v>
-      </c>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="47">
-        <v>0</v>
-      </c>
-      <c r="R20" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="48">
-        <v>4</v>
-      </c>
-      <c r="L21" s="48">
-        <v>4</v>
-      </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="47">
-        <v>0</v>
-      </c>
-      <c r="R21" s="47">
+      <c r="O35" s="47"/>
+      <c r="P35" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="47">
+        <v>0</v>
+      </c>
+      <c r="R35" s="47">
         <v>1</v>
       </c>
     </row>
@@ -2695,10 +3185,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2713,7 +3203,7 @@
     <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2757,27 +3247,24 @@
         <v>49</v>
       </c>
       <c r="O1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="P1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
         <v>61</v>
@@ -2809,22 +3296,19 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
@@ -2856,72 +3340,63 @@
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:16" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="F4" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="48">
+        <v>5</v>
+      </c>
+      <c r="J4" s="48">
+        <v>5</v>
+      </c>
+      <c r="L4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N4" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="49">
+        <v>1</v>
+      </c>
+      <c r="P4" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>61</v>
@@ -2936,13 +3411,13 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
         <v>2</v>
@@ -2956,22 +3431,19 @@
       <c r="P5">
         <v>1</v>
       </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>61</v>
@@ -2986,13 +3458,13 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="J6">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="L6" t="s">
         <v>2</v>
@@ -3006,7 +3478,339 @@
       <c r="P6">
         <v>1</v>
       </c>
-      <c r="Q6">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>21</v>
+      </c>
+      <c r="J7">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="49">
+        <v>2</v>
+      </c>
+      <c r="J8" s="49">
+        <v>2</v>
+      </c>
+      <c r="K8" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="49">
+        <v>1</v>
+      </c>
+      <c r="P8" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="49">
+        <v>12</v>
+      </c>
+      <c r="J9" s="49">
+        <v>12</v>
+      </c>
+      <c r="K9" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="49">
+        <v>1</v>
+      </c>
+      <c r="P9" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="49">
+        <v>22</v>
+      </c>
+      <c r="J10" s="49">
+        <v>22</v>
+      </c>
+      <c r="K10" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="49">
+        <v>1</v>
+      </c>
+      <c r="P10" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="49">
+        <v>4</v>
+      </c>
+      <c r="J11" s="49">
+        <v>4</v>
+      </c>
+      <c r="K11" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="49">
+        <v>1</v>
+      </c>
+      <c r="P11" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="49">
+        <v>14</v>
+      </c>
+      <c r="J12" s="49">
+        <v>14</v>
+      </c>
+      <c r="K12" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="49">
+        <v>1</v>
+      </c>
+      <c r="P12" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="49">
+        <v>24</v>
+      </c>
+      <c r="J13" s="49">
+        <v>24</v>
+      </c>
+      <c r="K13" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="49">
+        <v>1</v>
+      </c>
+      <c r="P13" s="49">
         <v>1</v>
       </c>
     </row>
@@ -3713,7 +4517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AF7103-8857-48FF-AABC-4046A666E527}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3724,19 +4528,19 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -3744,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D2">
         <v>794</v>
@@ -3761,10 +4565,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D3">
         <v>1280</v>
@@ -3781,10 +4585,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D4">
         <v>794</v>
@@ -3802,6 +4606,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100983CA113FD3DE849936E610BB0BA65BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="219e2d0d25f1c7dcecf6ea1ad6d45ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="75aa8e05-1f40-4a55-97cf-096775f63a7d" xmlns:ns4="c8ed7201-aa74-4219-b068-ce108ea8c5d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="719f9bc1c175b59cc8afcdde64e7182e" ns3:_="" ns4:_="">
     <xsd:import namespace="75aa8e05-1f40-4a55-97cf-096775f63a7d"/>
@@ -4010,22 +4823,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{985D8399-A071-4822-87D9-C2DF6320BB4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F60B9C7-E153-401A-BDEA-AEEC941471A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4044,7 +4856,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F429AA-8564-4E9A-81C4-E2167E53561A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4059,12 +4871,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{985D8399-A071-4822-87D9-C2DF6320BB4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Timeseries example data and readme updates
</commit_message>
<xml_diff>
--- a/Example/Example_project/Info2.xlsx
+++ b/Example/Example_project/Info2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nms198_newcastle_ac_uk/Documents/3_Coding/Git/TimeSeriesProcessor/Example/Example_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="923" documentId="6_{9E37F347-3A89-43C3-83FF-EA444BC37A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{921CC7AC-E0F1-4630-BAE6-2EF8615FCA49}"/>
+  <xr:revisionPtr revIDLastSave="925" documentId="6_{9E37F347-3A89-43C3-83FF-EA444BC37A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B402C71-49A8-4C86-B9A2-133886740026}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="713" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="9" r:id="rId1"/>
@@ -257,12 +257,6 @@
     <t>circle</t>
   </si>
   <si>
-    <t>BOD₅ (mg/l O₂)</t>
-  </si>
-  <si>
-    <t>COD (mg/l O₂)</t>
-  </si>
-  <si>
     <t>EVENTS</t>
   </si>
   <si>
@@ -702,6 +696,12 @@
   </si>
   <si>
     <t>Example/Example_Sample_data/</t>
+  </si>
+  <si>
+    <t>COD&lt;br&gt;(mg/l O₂)</t>
+  </si>
+  <si>
+    <t>BOD₅&lt;br&gt;(mg/l O₂)</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1310,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1331,7 +1331,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -1355,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1396,13 +1396,13 @@
     </row>
     <row r="2" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="37">
         <v>1</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E2" s="39" t="s">
         <v>23</v>
@@ -1413,13 +1413,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -1470,22 +1470,22 @@
         <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>89</v>
-      </c>
-      <c r="K1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -1525,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1557,10 +1557,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -1591,10 +1591,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" s="42">
         <v>44566.375</v>
@@ -1629,7 +1629,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1700,18 +1700,18 @@
         <v>58</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1768,10 +1768,10 @@
     </row>
     <row r="5" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
@@ -1781,7 +1781,7 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>217</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1804,7 +1804,7 @@
         <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>218</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1850,10 +1850,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
         <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>74</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -1964,30 +1964,30 @@
         <v>49</v>
       </c>
       <c r="Q1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
@@ -2022,22 +2022,22 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
         <v>61</v>
@@ -2072,22 +2072,22 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G4" t="s">
         <v>61</v>
@@ -2122,22 +2122,22 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
         <v>61</v>
@@ -2172,22 +2172,22 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C6" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="47" t="s">
-        <v>140</v>
-      </c>
       <c r="E6" s="49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
@@ -2222,22 +2222,22 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="47" t="s">
-        <v>141</v>
-      </c>
       <c r="E7" s="49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
         <v>61</v>
@@ -2272,19 +2272,19 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
@@ -2298,19 +2298,19 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
         <v>65</v>
@@ -2324,19 +2324,19 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F10" t="s">
         <v>65</v>
@@ -2350,19 +2350,19 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
         <v>67</v>
@@ -2376,19 +2376,19 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
         <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F12" t="s">
         <v>67</v>
@@ -2402,19 +2402,19 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F13" t="s">
         <v>67</v>
@@ -2428,19 +2428,19 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F14" t="s">
         <v>67</v>
@@ -2454,19 +2454,19 @@
     </row>
     <row r="15" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B15" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F15" s="49" t="s">
         <v>65</v>
@@ -2480,19 +2480,19 @@
     </row>
     <row r="16" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F16" s="49" t="s">
         <v>65</v>
@@ -2506,19 +2506,19 @@
     </row>
     <row r="17" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B17" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F17" s="49" t="s">
         <v>65</v>
@@ -2532,19 +2532,19 @@
     </row>
     <row r="18" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="49" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F18" s="49" t="s">
         <v>67</v>
@@ -2558,19 +2558,19 @@
     </row>
     <row r="19" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" s="49" t="s">
         <v>66</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F19" s="49" t="s">
         <v>67</v>
@@ -2584,19 +2584,19 @@
     </row>
     <row r="20" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F20" s="49" t="s">
         <v>67</v>
@@ -2610,19 +2610,19 @@
     </row>
     <row r="21" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B21" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F21" s="49" t="s">
         <v>67</v>
@@ -2636,19 +2636,19 @@
     </row>
     <row r="22" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B22" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F22" s="49" t="s">
         <v>65</v>
@@ -2662,19 +2662,19 @@
     </row>
     <row r="23" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F23" s="49" t="s">
         <v>65</v>
@@ -2688,19 +2688,19 @@
     </row>
     <row r="24" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B24" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F24" s="49" t="s">
         <v>65</v>
@@ -2714,19 +2714,19 @@
     </row>
     <row r="25" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B25" s="49" t="s">
         <v>66</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F25" s="49" t="s">
         <v>67</v>
@@ -2740,19 +2740,19 @@
     </row>
     <row r="26" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B26" s="49" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F26" s="49" t="s">
         <v>67</v>
@@ -2766,19 +2766,19 @@
     </row>
     <row r="27" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B27" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F27" s="49" t="s">
         <v>67</v>
@@ -2792,19 +2792,19 @@
     </row>
     <row r="28" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B28" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E28" s="49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F28" s="49" t="s">
         <v>67</v>
@@ -2818,25 +2818,25 @@
     </row>
     <row r="29" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E29" s="46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F29" s="46" t="s">
         <v>43</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H29" s="49" t="b">
         <v>0</v>
@@ -2870,22 +2870,22 @@
     </row>
     <row r="30" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F30" s="44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44" t="b">
@@ -2922,22 +2922,22 @@
     </row>
     <row r="31" spans="1:18" s="47" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H31" s="47" t="b">
         <v>0</v>
@@ -2972,22 +2972,22 @@
     </row>
     <row r="32" spans="1:18" s="47" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H32" s="47" t="b">
         <v>0</v>
@@ -3022,19 +3022,19 @@
     </row>
     <row r="33" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E33" s="47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F33" s="47" t="s">
         <v>43</v>
@@ -3074,19 +3074,19 @@
     </row>
     <row r="34" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C34" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="47" t="s">
-        <v>133</v>
-      </c>
       <c r="E34" s="47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F34" s="47" t="s">
         <v>43</v>
@@ -3126,19 +3126,19 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F35" s="47" t="s">
         <v>43</v>
@@ -3247,24 +3247,24 @@
         <v>49</v>
       </c>
       <c r="O1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
         <v>61</v>
@@ -3299,16 +3299,16 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
@@ -3343,13 +3343,13 @@
     </row>
     <row r="4" spans="1:16" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>43</v>
@@ -3387,13 +3387,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s">
         <v>65</v>
@@ -3434,13 +3434,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
         <v>67</v>
@@ -3481,13 +3481,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
         <v>67</v>
@@ -3528,13 +3528,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D8" s="49" t="s">
         <v>65</v>
@@ -3576,13 +3576,13 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D9" s="49" t="s">
         <v>67</v>
@@ -3624,13 +3624,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D10" s="49" t="s">
         <v>67</v>
@@ -3672,13 +3672,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D11" s="49" t="s">
         <v>65</v>
@@ -3720,13 +3720,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D12" s="49" t="s">
         <v>67</v>
@@ -3768,13 +3768,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="49" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D13" s="49" t="s">
         <v>67</v>
@@ -4528,19 +4528,19 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4548,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2">
         <v>794</v>
@@ -4565,10 +4565,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3">
         <v>1280</v>
@@ -4585,10 +4585,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>794</v>
@@ -4606,9 +4606,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4821,27 +4824,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F429AA-8564-4E9A-81C4-E2167E53561A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{985D8399-A071-4822-87D9-C2DF6320BB4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="75aa8e05-1f40-4a55-97cf-096775f63a7d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c8ed7201-aa74-4219-b068-ce108ea8c5d8"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4866,9 +4857,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{985D8399-A071-4822-87D9-C2DF6320BB4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F429AA-8564-4E9A-81C4-E2167E53561A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="75aa8e05-1f40-4a55-97cf-096775f63a7d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c8ed7201-aa74-4219-b068-ce108ea8c5d8"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>